<commit_message>
updated data post lab meeting
</commit_message>
<xml_diff>
--- a/data/historical-distributions.xlsx
+++ b/data/historical-distributions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="372">
   <si>
     <t>latin_name</t>
   </si>
@@ -1592,6 +1592,9 @@
     <t>Pyrosoma sp.</t>
   </si>
   <si>
+    <t>Pyrosoma</t>
+  </si>
+  <si>
     <t>Rhincalanus nasutus</t>
   </si>
   <si>
@@ -1729,6 +1732,9 @@
   </si>
   <si>
     <t>cosmopolitan species</t>
+  </si>
+  <si>
+    <t>Thetys</t>
   </si>
   <si>
     <t>Uca princeps</t>
@@ -1876,6 +1882,9 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Velella</t>
+  </si>
+  <si>
+    <t>Velella</t>
   </si>
   <si>
     <t>Books</t>
@@ -5643,8 +5652,12 @@
       <c r="D102" s="10">
         <v>36.78</v>
       </c>
-      <c r="E102" s="3"/>
-      <c r="F102" s="3"/>
+      <c r="E102" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F102" s="2">
+        <v>948.0</v>
+      </c>
       <c r="G102" s="2" t="s">
         <v>165</v>
       </c>
@@ -6144,29 +6157,30 @@
       <c r="S122" s="3"/>
     </row>
     <row r="123">
-      <c r="A123" s="1" t="s">
+      <c r="A123" s="2" t="s">
         <v>314</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C123" s="34" t="s">
-        <v>315</v>
-      </c>
-      <c r="D123" s="2"/>
+        <v>309</v>
+      </c>
+      <c r="C123" s="43" t="s">
+        <v>310</v>
+      </c>
+      <c r="D123" s="2">
+        <v>40.0</v>
+      </c>
       <c r="E123" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F123" s="3"/>
-      <c r="G123" s="3"/>
-      <c r="H123" s="9" t="s">
-        <v>316</v>
+      <c r="H123" s="41" t="s">
+        <v>311</v>
       </c>
       <c r="I123" s="3"/>
       <c r="J123" s="3"/>
       <c r="K123" s="3"/>
       <c r="L123" s="3"/>
-      <c r="M123" s="2"/>
+      <c r="M123" s="3"/>
       <c r="N123" s="3"/>
       <c r="O123" s="3"/>
       <c r="P123" s="3"/>
@@ -6176,24 +6190,22 @@
     </row>
     <row r="124">
       <c r="A124" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C124" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="D124" s="2">
-        <v>34.5</v>
-      </c>
+      <c r="C124" s="34" t="s">
+        <v>316</v>
+      </c>
+      <c r="D124" s="2"/>
       <c r="E124" s="2" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="F124" s="3"/>
       <c r="G124" s="3"/>
       <c r="H124" s="9" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="I124" s="3"/>
       <c r="J124" s="3"/>
@@ -6209,22 +6221,24 @@
     </row>
     <row r="125">
       <c r="A125" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C125" s="44" t="s">
-        <v>318</v>
-      </c>
-      <c r="D125" s="2"/>
+      <c r="C125" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D125" s="2">
+        <v>34.5</v>
+      </c>
       <c r="E125" s="2" t="s">
-        <v>319</v>
+        <v>57</v>
       </c>
       <c r="F125" s="3"/>
       <c r="G125" s="3"/>
       <c r="H125" s="9" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="I125" s="3"/>
       <c r="J125" s="3"/>
@@ -6239,94 +6253,93 @@
       <c r="S125" s="3"/>
     </row>
     <row r="126">
-      <c r="A126" s="45" t="s">
-        <v>317</v>
-      </c>
-      <c r="B126" s="22" t="s">
+      <c r="A126" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B126" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C126" s="7" t="s">
+      <c r="C126" s="44" t="s">
+        <v>319</v>
+      </c>
+      <c r="D126" s="2"/>
+      <c r="E126" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="F126" s="3"/>
+      <c r="G126" s="3"/>
+      <c r="H126" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="D126" s="8">
+      <c r="I126" s="3"/>
+      <c r="J126" s="3"/>
+      <c r="K126" s="3"/>
+      <c r="L126" s="3"/>
+      <c r="M126" s="2"/>
+      <c r="N126" s="3"/>
+      <c r="O126" s="3"/>
+      <c r="P126" s="3"/>
+      <c r="Q126" s="3"/>
+      <c r="R126" s="3"/>
+      <c r="S126" s="3"/>
+    </row>
+    <row r="127">
+      <c r="A127" s="45" t="s">
+        <v>318</v>
+      </c>
+      <c r="B127" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C127" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="D127" s="8">
         <v>42.0</v>
       </c>
-      <c r="E126" s="8" t="s">
+      <c r="E127" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G126" s="26"/>
-      <c r="H126" s="25" t="s">
-        <v>320</v>
-      </c>
-      <c r="I126" s="26"/>
-      <c r="J126" s="26"/>
-      <c r="K126" s="26"/>
-      <c r="L126" s="26"/>
-      <c r="M126" s="22"/>
-      <c r="N126" s="26"/>
-      <c r="O126" s="26"/>
-      <c r="P126" s="26"/>
-      <c r="Q126" s="26"/>
-      <c r="R126" s="26"/>
-      <c r="S126" s="26"/>
-      <c r="T126" s="26"/>
-      <c r="U126" s="26"/>
-      <c r="V126" s="26"/>
-      <c r="W126" s="26"/>
-      <c r="X126" s="26"/>
-      <c r="Y126" s="26"/>
-      <c r="Z126" s="26"/>
-    </row>
-    <row r="127">
-      <c r="A127" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C127" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="D127" s="2"/>
-      <c r="E127" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="F127" s="3"/>
-      <c r="G127" s="3"/>
-      <c r="H127" s="9" t="s">
-        <v>325</v>
-      </c>
-      <c r="I127" s="3"/>
-      <c r="J127" s="3"/>
-      <c r="K127" s="3"/>
-      <c r="L127" s="3"/>
-      <c r="N127" s="3"/>
-      <c r="O127" s="3"/>
-      <c r="P127" s="3"/>
-      <c r="Q127" s="3"/>
-      <c r="R127" s="3"/>
-      <c r="S127" s="3"/>
+      <c r="G127" s="26"/>
+      <c r="H127" s="25" t="s">
+        <v>321</v>
+      </c>
+      <c r="I127" s="26"/>
+      <c r="J127" s="26"/>
+      <c r="K127" s="26"/>
+      <c r="L127" s="26"/>
+      <c r="M127" s="22"/>
+      <c r="N127" s="26"/>
+      <c r="O127" s="26"/>
+      <c r="P127" s="26"/>
+      <c r="Q127" s="26"/>
+      <c r="R127" s="26"/>
+      <c r="S127" s="26"/>
+      <c r="T127" s="26"/>
+      <c r="U127" s="26"/>
+      <c r="V127" s="26"/>
+      <c r="W127" s="26"/>
+      <c r="X127" s="26"/>
+      <c r="Y127" s="26"/>
+      <c r="Z127" s="26"/>
     </row>
     <row r="128">
       <c r="A128" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D128" s="2">
-        <v>34.5</v>
-      </c>
+        <v>324</v>
+      </c>
+      <c r="D128" s="2"/>
       <c r="E128" s="2" t="s">
-        <v>57</v>
+        <v>325</v>
       </c>
       <c r="F128" s="3"/>
       <c r="G128" s="3"/>
       <c r="H128" s="9" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="I128" s="3"/>
       <c r="J128" s="3"/>
@@ -6341,32 +6354,29 @@
     </row>
     <row r="129">
       <c r="A129" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>327</v>
+        <v>55</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>328</v>
+        <v>56</v>
       </c>
       <c r="D129" s="2">
         <v>34.5</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F129" s="2">
-        <v>735.0</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="F129" s="3"/>
       <c r="G129" s="3"/>
       <c r="H129" s="9" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="I129" s="3"/>
       <c r="J129" s="3"/>
       <c r="K129" s="3"/>
       <c r="L129" s="3"/>
-      <c r="M129" s="2"/>
       <c r="N129" s="3"/>
       <c r="O129" s="3"/>
       <c r="P129" s="3"/>
@@ -6376,24 +6386,26 @@
     </row>
     <row r="130">
       <c r="A130" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="D130" s="1"/>
-      <c r="E130" s="1" t="s">
-        <v>12</v>
+        <v>329</v>
+      </c>
+      <c r="D130" s="2">
+        <v>34.5</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="F130" s="2">
-        <v>68.0</v>
+        <v>735.0</v>
       </c>
       <c r="G130" s="3"/>
       <c r="H130" s="9" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="I130" s="3"/>
       <c r="J130" s="3"/>
@@ -6409,28 +6421,30 @@
     </row>
     <row r="131">
       <c r="A131" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C131" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="B131" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="C131" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="D131" s="2"/>
-      <c r="E131" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F131" s="3"/>
+      <c r="D131" s="1"/>
+      <c r="E131" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F131" s="2">
+        <v>68.0</v>
+      </c>
       <c r="G131" s="3"/>
       <c r="H131" s="9" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="I131" s="3"/>
       <c r="J131" s="3"/>
       <c r="K131" s="3"/>
       <c r="L131" s="3"/>
-      <c r="M131" s="3"/>
+      <c r="M131" s="2"/>
       <c r="N131" s="3"/>
       <c r="O131" s="3"/>
       <c r="P131" s="3"/>
@@ -6440,23 +6454,22 @@
     </row>
     <row r="132">
       <c r="A132" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="C132" s="46" t="s">
-        <v>336</v>
-      </c>
-      <c r="D132" s="10">
-        <v>36.0</v>
-      </c>
-      <c r="E132" s="8" t="s">
-        <v>14</v>
-      </c>
+        <v>334</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D132" s="2"/>
+      <c r="E132" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F132" s="3"/>
       <c r="G132" s="3"/>
       <c r="H132" s="9" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="I132" s="3"/>
       <c r="J132" s="3"/>
@@ -6472,26 +6485,23 @@
     </row>
     <row r="133">
       <c r="A133" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C133" s="46" t="s">
         <v>337</v>
       </c>
-      <c r="B133" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="C133" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="D133" s="11">
-        <v>37.5</v>
-      </c>
-      <c r="E133" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F133" s="2">
-        <v>482.0</v>
+      <c r="D133" s="10">
+        <v>36.0</v>
+      </c>
+      <c r="E133" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="G133" s="3"/>
       <c r="H133" s="9" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="I133" s="3"/>
       <c r="J133" s="3"/>
@@ -6507,22 +6517,26 @@
     </row>
     <row r="134">
       <c r="A134" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="C134" s="47" t="s">
-        <v>341</v>
-      </c>
-      <c r="D134" s="2"/>
+        <v>339</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="D134" s="11">
+        <v>37.5</v>
+      </c>
       <c r="E134" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="F134" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="F134" s="2">
+        <v>482.0</v>
+      </c>
       <c r="G134" s="3"/>
       <c r="H134" s="9" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="I134" s="3"/>
       <c r="J134" s="3"/>
@@ -6538,22 +6552,22 @@
     </row>
     <row r="135">
       <c r="A135" s="1" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C135" s="39" t="s">
-        <v>344</v>
+        <v>339</v>
+      </c>
+      <c r="C135" s="47" t="s">
+        <v>342</v>
       </c>
       <c r="D135" s="2"/>
       <c r="E135" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F135" s="3"/>
+        <v>343</v>
+      </c>
+      <c r="F135" s="2"/>
       <c r="G135" s="3"/>
       <c r="H135" s="9" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="I135" s="3"/>
       <c r="J135" s="3"/>
@@ -6569,24 +6583,22 @@
     </row>
     <row r="136">
       <c r="A136" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C136" s="39" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D136" s="2"/>
       <c r="E136" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F136" s="2">
-        <v>82.0</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="F136" s="3"/>
       <c r="G136" s="3"/>
       <c r="H136" s="9" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="I136" s="3"/>
       <c r="J136" s="3"/>
@@ -6602,22 +6614,24 @@
     </row>
     <row r="137">
       <c r="A137" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C137" s="48" t="s">
+      <c r="C137" s="39" t="s">
         <v>347</v>
       </c>
-      <c r="D137" s="2">
-        <v>35.0</v>
-      </c>
-      <c r="E137" s="2"/>
-      <c r="F137" s="2"/>
+      <c r="D137" s="2"/>
+      <c r="E137" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F137" s="2">
+        <v>82.0</v>
+      </c>
       <c r="G137" s="3"/>
       <c r="H137" s="9" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="I137" s="3"/>
       <c r="J137" s="3"/>
@@ -6633,24 +6647,22 @@
     </row>
     <row r="138">
       <c r="A138" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C138" s="48" t="s">
         <v>348</v>
       </c>
-      <c r="B138" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="D138" s="2"/>
-      <c r="E138" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F138" s="2">
-        <v>82.0</v>
-      </c>
+      <c r="D138" s="2">
+        <v>35.0</v>
+      </c>
+      <c r="E138" s="2"/>
+      <c r="F138" s="2"/>
       <c r="G138" s="3"/>
       <c r="H138" s="9" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="I138" s="3"/>
       <c r="J138" s="3"/>
@@ -6666,24 +6678,24 @@
     </row>
     <row r="139">
       <c r="A139" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D139" s="2"/>
       <c r="E139" s="2" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="F139" s="2">
-        <v>964.0</v>
+        <v>82.0</v>
       </c>
       <c r="G139" s="3"/>
       <c r="H139" s="9" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="I139" s="3"/>
       <c r="J139" s="3"/>
@@ -6699,17 +6711,15 @@
     </row>
     <row r="140">
       <c r="A140" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="C140" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="C140" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="D140" s="2">
-        <v>42.0</v>
-      </c>
+      <c r="D140" s="2"/>
       <c r="E140" s="2" t="s">
         <v>29</v>
       </c>
@@ -6718,7 +6728,7 @@
       </c>
       <c r="G140" s="3"/>
       <c r="H140" s="9" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="I140" s="3"/>
       <c r="J140" s="3"/>
@@ -6734,22 +6744,26 @@
     </row>
     <row r="141">
       <c r="A141" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C141" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="B141" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="C141" s="40" t="s">
-        <v>356</v>
-      </c>
-      <c r="D141" s="2"/>
+      <c r="D141" s="2">
+        <v>42.0</v>
+      </c>
       <c r="E141" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F141" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="F141" s="2">
+        <v>964.0</v>
+      </c>
       <c r="G141" s="3"/>
       <c r="H141" s="9" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="I141" s="3"/>
       <c r="J141" s="3"/>
@@ -6764,25 +6778,27 @@
       <c r="S141" s="3"/>
     </row>
     <row r="142">
-      <c r="A142" s="1" t="s">
+      <c r="A142" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C142" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="B142" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="C142" s="35" t="s">
-        <v>358</v>
-      </c>
       <c r="D142" s="2">
-        <v>22.8</v>
-      </c>
-      <c r="E142" s="30" t="s">
-        <v>359</v>
-      </c>
-      <c r="F142" s="3"/>
+        <v>42.0</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F142" s="2">
+        <v>964.0</v>
+      </c>
       <c r="G142" s="3"/>
       <c r="H142" s="9" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="I142" s="3"/>
       <c r="J142" s="3"/>
@@ -6798,26 +6814,22 @@
     </row>
     <row r="143">
       <c r="A143" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="C143" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="D143" s="2">
-        <v>34.5</v>
-      </c>
+        <v>357</v>
+      </c>
+      <c r="C143" s="40" t="s">
+        <v>358</v>
+      </c>
+      <c r="D143" s="2"/>
       <c r="E143" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F143" s="2">
-        <v>31.0</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F143" s="3"/>
       <c r="G143" s="3"/>
       <c r="H143" s="9" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="I143" s="3"/>
       <c r="J143" s="3"/>
@@ -6832,14 +6844,26 @@
       <c r="S143" s="3"/>
     </row>
     <row r="144">
-      <c r="A144" s="3"/>
-      <c r="B144" s="3"/>
-      <c r="C144" s="3"/>
-      <c r="D144" s="3"/>
-      <c r="E144" s="3"/>
+      <c r="A144" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C144" s="35" t="s">
+        <v>360</v>
+      </c>
+      <c r="D144" s="2">
+        <v>22.8</v>
+      </c>
+      <c r="E144" s="30" t="s">
+        <v>361</v>
+      </c>
       <c r="F144" s="3"/>
       <c r="G144" s="3"/>
-      <c r="H144" s="3"/>
+      <c r="H144" s="9" t="s">
+        <v>359</v>
+      </c>
       <c r="I144" s="3"/>
       <c r="J144" s="3"/>
       <c r="K144" s="3"/>
@@ -6853,14 +6877,28 @@
       <c r="S144" s="3"/>
     </row>
     <row r="145">
-      <c r="A145" s="3"/>
-      <c r="B145" s="3"/>
-      <c r="C145" s="3"/>
-      <c r="D145" s="3"/>
-      <c r="E145" s="3"/>
-      <c r="F145" s="3"/>
+      <c r="A145" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="D145" s="2">
+        <v>34.5</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F145" s="2">
+        <v>31.0</v>
+      </c>
       <c r="G145" s="3"/>
-      <c r="H145" s="3"/>
+      <c r="H145" s="9" t="s">
+        <v>365</v>
+      </c>
       <c r="I145" s="3"/>
       <c r="J145" s="3"/>
       <c r="K145" s="3"/>
@@ -6874,14 +6912,28 @@
       <c r="S145" s="3"/>
     </row>
     <row r="146">
-      <c r="A146" s="3"/>
-      <c r="B146" s="3"/>
-      <c r="C146" s="3"/>
-      <c r="D146" s="3"/>
-      <c r="E146" s="3"/>
-      <c r="F146" s="3"/>
+      <c r="A146" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="D146" s="2">
+        <v>34.5</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F146" s="2">
+        <v>31.0</v>
+      </c>
       <c r="G146" s="3"/>
-      <c r="H146" s="3"/>
+      <c r="H146" s="9" t="s">
+        <v>365</v>
+      </c>
       <c r="I146" s="3"/>
       <c r="J146" s="3"/>
       <c r="K146" s="3"/>
@@ -6914,6 +6966,48 @@
       <c r="Q147" s="3"/>
       <c r="R147" s="3"/>
       <c r="S147" s="3"/>
+    </row>
+    <row r="148">
+      <c r="A148" s="3"/>
+      <c r="B148" s="3"/>
+      <c r="C148" s="3"/>
+      <c r="D148" s="3"/>
+      <c r="E148" s="3"/>
+      <c r="F148" s="3"/>
+      <c r="G148" s="3"/>
+      <c r="H148" s="3"/>
+      <c r="I148" s="3"/>
+      <c r="J148" s="3"/>
+      <c r="K148" s="3"/>
+      <c r="L148" s="3"/>
+      <c r="M148" s="3"/>
+      <c r="N148" s="3"/>
+      <c r="O148" s="3"/>
+      <c r="P148" s="3"/>
+      <c r="Q148" s="3"/>
+      <c r="R148" s="3"/>
+      <c r="S148" s="3"/>
+    </row>
+    <row r="149">
+      <c r="A149" s="3"/>
+      <c r="B149" s="3"/>
+      <c r="C149" s="3"/>
+      <c r="D149" s="3"/>
+      <c r="E149" s="3"/>
+      <c r="F149" s="3"/>
+      <c r="G149" s="3"/>
+      <c r="H149" s="3"/>
+      <c r="I149" s="3"/>
+      <c r="J149" s="3"/>
+      <c r="K149" s="3"/>
+      <c r="L149" s="3"/>
+      <c r="M149" s="3"/>
+      <c r="N149" s="3"/>
+      <c r="O149" s="3"/>
+      <c r="P149" s="3"/>
+      <c r="Q149" s="3"/>
+      <c r="R149" s="3"/>
+      <c r="S149" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="116">
@@ -6981,8 +7075,8 @@
     <mergeCell ref="H85:T85"/>
     <mergeCell ref="E90:F90"/>
     <mergeCell ref="E113:F113"/>
-    <mergeCell ref="E126:F126"/>
-    <mergeCell ref="E132:F132"/>
+    <mergeCell ref="E127:F127"/>
+    <mergeCell ref="E133:F133"/>
     <mergeCell ref="E96:F96"/>
     <mergeCell ref="E98:F98"/>
     <mergeCell ref="E101:F101"/>
@@ -7158,8 +7252,8 @@
     <hyperlink r:id="rId121" ref="H120"/>
     <hyperlink r:id="rId122" ref="H121"/>
     <hyperlink r:id="rId123" ref="H122"/>
-    <hyperlink r:id="rId124" ref="C123"/>
-    <hyperlink r:id="rId125" ref="H123"/>
+    <hyperlink r:id="rId124" ref="H123"/>
+    <hyperlink r:id="rId125" ref="C124"/>
     <hyperlink r:id="rId126" ref="H124"/>
     <hyperlink r:id="rId127" ref="H125"/>
     <hyperlink r:id="rId128" ref="H126"/>
@@ -7177,13 +7271,16 @@
     <hyperlink r:id="rId140" ref="H138"/>
     <hyperlink r:id="rId141" ref="H139"/>
     <hyperlink r:id="rId142" ref="H140"/>
-    <hyperlink r:id="rId143" ref="C141"/>
-    <hyperlink r:id="rId144" ref="H141"/>
-    <hyperlink r:id="rId145" ref="E142"/>
-    <hyperlink r:id="rId146" ref="H142"/>
-    <hyperlink r:id="rId147" ref="H143"/>
+    <hyperlink r:id="rId143" ref="H141"/>
+    <hyperlink r:id="rId144" ref="H142"/>
+    <hyperlink r:id="rId145" ref="C143"/>
+    <hyperlink r:id="rId146" ref="H143"/>
+    <hyperlink r:id="rId147" ref="E144"/>
+    <hyperlink r:id="rId148" ref="H144"/>
+    <hyperlink r:id="rId149" ref="H145"/>
+    <hyperlink r:id="rId150" ref="H146"/>
   </hyperlinks>
-  <drawing r:id="rId148"/>
+  <drawing r:id="rId151"/>
 </worksheet>
 </file>
 
@@ -7199,15 +7296,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="3">
@@ -7227,12 +7324,12 @@
     </row>
     <row r="6">
       <c r="A6" s="30" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="30" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
fixed the dubious species latitude 2b conservative
</commit_message>
<xml_diff>
--- a/data/historical-distributions.xlsx
+++ b/data/historical-distributions.xlsx
@@ -47,7 +47,7 @@
     <t>American seashells</t>
   </si>
   <si>
-    <t>may have gotten mixed up with acanthina punctulata</t>
+    <t>may have gotten mixed up with acanthina punctulata (would have range edge of 38.1 if that's the case)</t>
   </si>
   <si>
     <t>Field Guid to Pacific Coast Shells</t>
@@ -1957,8 +1957,9 @@
     </font>
     <font>
       <sz val="12.0"/>
-      <color rgb="FF9900FF"/>
-      <name val="&quot;Aptos Narrow&quot;"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12.0"/>
@@ -2083,7 +2084,7 @@
     </font>
     <font>
       <sz val="12.0"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="&quot;Aptos Narrow&quot;"/>
     </font>
     <font>
@@ -2174,11 +2175,11 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -2571,7 +2572,7 @@
       <c r="R1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2584,7 +2585,7 @@
       <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>211.0</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -2600,7 +2601,7 @@
       <c r="R2" s="3"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -2609,7 +2610,9 @@
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="5">
+        <v>47.72</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
@@ -2629,7 +2632,7 @@
       <c r="R3" s="3"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -2638,9 +2641,7 @@
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="7">
-        <v>38.1</v>
-      </c>
+      <c r="D4" s="7"/>
       <c r="E4" s="8" t="s">
         <v>14</v>
       </c>
@@ -2956,7 +2957,7 @@
       <c r="E14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <v>485.0</v>
       </c>
       <c r="G14" s="3"/>
@@ -4412,7 +4413,7 @@
       <c r="E62" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F62" s="5">
+      <c r="F62" s="4">
         <v>176.0</v>
       </c>
       <c r="G62" s="2" t="s">
@@ -4746,7 +4747,7 @@
       <c r="E73" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F73" s="5">
+      <c r="F73" s="4">
         <v>97.0</v>
       </c>
       <c r="G73" s="1" t="s">
@@ -4874,7 +4875,7 @@
       <c r="E77" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F77" s="5">
+      <c r="F77" s="4">
         <v>482.0</v>
       </c>
       <c r="G77" s="3"/>
@@ -4902,7 +4903,7 @@
       <c r="E78" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="F78" s="5"/>
+      <c r="F78" s="4"/>
       <c r="G78" s="3"/>
       <c r="H78" s="9" t="s">
         <v>201</v>
@@ -5043,7 +5044,7 @@
       <c r="E83" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F83" s="5">
+      <c r="F83" s="4">
         <v>128.0</v>
       </c>
       <c r="G83" s="1" t="s">

</xml_diff>

<commit_message>
fixed an na and wiki resource
</commit_message>
<xml_diff>
--- a/data/historical-distributions.xlsx
+++ b/data/historical-distributions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="371">
   <si>
     <t>latin_name</t>
   </si>
@@ -1587,9 +1587,6 @@
   </si>
   <si>
     <t>tropical and temperate Atlantic, Pacific, and Indian Oceans</t>
-  </si>
-  <si>
-    <t>Pyrosoma sp.</t>
   </si>
   <si>
     <t>Pyrosoma</t>
@@ -1938,7 +1935,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="39">
+  <fonts count="38">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -2123,11 +2120,6 @@
       <name val="&quot;Open Sans&quot;"/>
     </font>
     <font>
-      <sz val="12.0"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-    </font>
-    <font>
       <color rgb="FF111111"/>
       <name val="Arial"/>
     </font>
@@ -2298,16 +2290,16 @@
     <xf borderId="0" fillId="2" fontId="34" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="36" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="37" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="36" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="38" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="37" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -6126,22 +6118,24 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="1" t="s">
+      <c r="A122" s="2" t="s">
         <v>313</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="C122" s="43" t="s">
-        <v>310</v>
+      <c r="C122" s="35" t="s">
+        <v>312</v>
       </c>
       <c r="D122" s="2">
         <v>40.0</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F122" s="3"/>
+        <v>73</v>
+      </c>
+      <c r="F122" s="2">
+        <v>84.0</v>
+      </c>
       <c r="H122" s="41" t="s">
         <v>311</v>
       </c>
@@ -6158,30 +6152,29 @@
       <c r="S122" s="3"/>
     </row>
     <row r="123">
-      <c r="A123" s="2" t="s">
+      <c r="A123" s="1" t="s">
         <v>314</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="C123" s="43" t="s">
-        <v>310</v>
-      </c>
-      <c r="D123" s="2">
-        <v>40.0</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="C123" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="D123" s="2"/>
       <c r="E123" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F123" s="3"/>
-      <c r="H123" s="41" t="s">
-        <v>311</v>
+      <c r="G123" s="3"/>
+      <c r="H123" s="9" t="s">
+        <v>316</v>
       </c>
       <c r="I123" s="3"/>
       <c r="J123" s="3"/>
       <c r="K123" s="3"/>
       <c r="L123" s="3"/>
-      <c r="M123" s="3"/>
+      <c r="M123" s="2"/>
       <c r="N123" s="3"/>
       <c r="O123" s="3"/>
       <c r="P123" s="3"/>
@@ -6191,22 +6184,24 @@
     </row>
     <row r="124">
       <c r="A124" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C124" s="34" t="s">
-        <v>316</v>
-      </c>
-      <c r="D124" s="2"/>
+      <c r="C124" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D124" s="2">
+        <v>34.5</v>
+      </c>
       <c r="E124" s="2" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="F124" s="3"/>
       <c r="G124" s="3"/>
       <c r="H124" s="9" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I124" s="3"/>
       <c r="J124" s="3"/>
@@ -6222,24 +6217,22 @@
     </row>
     <row r="125">
       <c r="A125" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C125" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="D125" s="2">
-        <v>34.5</v>
-      </c>
+      <c r="C125" s="44" t="s">
+        <v>318</v>
+      </c>
+      <c r="D125" s="2"/>
       <c r="E125" s="2" t="s">
-        <v>57</v>
+        <v>319</v>
       </c>
       <c r="F125" s="3"/>
       <c r="G125" s="3"/>
       <c r="H125" s="9" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="I125" s="3"/>
       <c r="J125" s="3"/>
@@ -6254,93 +6247,94 @@
       <c r="S125" s="3"/>
     </row>
     <row r="126">
-      <c r="A126" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="B126" s="2" t="s">
+      <c r="A126" s="45" t="s">
+        <v>317</v>
+      </c>
+      <c r="B126" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C126" s="44" t="s">
-        <v>319</v>
-      </c>
-      <c r="D126" s="2"/>
-      <c r="E126" s="2" t="s">
+      <c r="C126" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="D126" s="8">
+        <v>42.0</v>
+      </c>
+      <c r="E126" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G126" s="26"/>
+      <c r="H126" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="F126" s="3"/>
-      <c r="G126" s="3"/>
-      <c r="H126" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="I126" s="3"/>
-      <c r="J126" s="3"/>
-      <c r="K126" s="3"/>
-      <c r="L126" s="3"/>
-      <c r="M126" s="2"/>
-      <c r="N126" s="3"/>
-      <c r="O126" s="3"/>
-      <c r="P126" s="3"/>
-      <c r="Q126" s="3"/>
-      <c r="R126" s="3"/>
-      <c r="S126" s="3"/>
+      <c r="I126" s="26"/>
+      <c r="J126" s="26"/>
+      <c r="K126" s="26"/>
+      <c r="L126" s="26"/>
+      <c r="M126" s="22"/>
+      <c r="N126" s="26"/>
+      <c r="O126" s="26"/>
+      <c r="P126" s="26"/>
+      <c r="Q126" s="26"/>
+      <c r="R126" s="26"/>
+      <c r="S126" s="26"/>
+      <c r="T126" s="26"/>
+      <c r="U126" s="26"/>
+      <c r="V126" s="26"/>
+      <c r="W126" s="26"/>
+      <c r="X126" s="26"/>
+      <c r="Y126" s="26"/>
+      <c r="Z126" s="26"/>
     </row>
     <row r="127">
-      <c r="A127" s="45" t="s">
-        <v>318</v>
-      </c>
-      <c r="B127" s="22" t="s">
+      <c r="A127" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B127" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C127" s="7" t="s">
-        <v>322</v>
-      </c>
-      <c r="D127" s="8">
-        <v>42.0</v>
-      </c>
-      <c r="E127" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G127" s="26"/>
-      <c r="H127" s="25" t="s">
-        <v>321</v>
-      </c>
-      <c r="I127" s="26"/>
-      <c r="J127" s="26"/>
-      <c r="K127" s="26"/>
-      <c r="L127" s="26"/>
-      <c r="M127" s="22"/>
-      <c r="N127" s="26"/>
-      <c r="O127" s="26"/>
-      <c r="P127" s="26"/>
-      <c r="Q127" s="26"/>
-      <c r="R127" s="26"/>
-      <c r="S127" s="26"/>
-      <c r="T127" s="26"/>
-      <c r="U127" s="26"/>
-      <c r="V127" s="26"/>
-      <c r="W127" s="26"/>
-      <c r="X127" s="26"/>
-      <c r="Y127" s="26"/>
-      <c r="Z127" s="26"/>
+      <c r="C127" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D127" s="2"/>
+      <c r="E127" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="F127" s="3"/>
+      <c r="G127" s="3"/>
+      <c r="H127" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="I127" s="3"/>
+      <c r="J127" s="3"/>
+      <c r="K127" s="3"/>
+      <c r="L127" s="3"/>
+      <c r="N127" s="3"/>
+      <c r="O127" s="3"/>
+      <c r="P127" s="3"/>
+      <c r="Q127" s="3"/>
+      <c r="R127" s="3"/>
+      <c r="S127" s="3"/>
     </row>
     <row r="128">
       <c r="A128" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="D128" s="2"/>
+        <v>56</v>
+      </c>
+      <c r="D128" s="2">
+        <v>34.5</v>
+      </c>
       <c r="E128" s="2" t="s">
-        <v>325</v>
+        <v>57</v>
       </c>
       <c r="F128" s="3"/>
       <c r="G128" s="3"/>
       <c r="H128" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I128" s="3"/>
       <c r="J128" s="3"/>
@@ -6355,29 +6349,32 @@
     </row>
     <row r="129">
       <c r="A129" s="1" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>55</v>
+        <v>327</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>56</v>
+        <v>328</v>
       </c>
       <c r="D129" s="2">
         <v>34.5</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F129" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="F129" s="2">
+        <v>735.0</v>
+      </c>
       <c r="G129" s="3"/>
       <c r="H129" s="9" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="I129" s="3"/>
       <c r="J129" s="3"/>
       <c r="K129" s="3"/>
       <c r="L129" s="3"/>
+      <c r="M129" s="2"/>
       <c r="N129" s="3"/>
       <c r="O129" s="3"/>
       <c r="P129" s="3"/>
@@ -6387,26 +6384,24 @@
     </row>
     <row r="130">
       <c r="A130" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="D130" s="2">
-        <v>34.5</v>
-      </c>
-      <c r="E130" s="2" t="s">
-        <v>29</v>
+        <v>331</v>
+      </c>
+      <c r="D130" s="1"/>
+      <c r="E130" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="F130" s="2">
-        <v>735.0</v>
+        <v>68.0</v>
       </c>
       <c r="G130" s="3"/>
       <c r="H130" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I130" s="3"/>
       <c r="J130" s="3"/>
@@ -6422,30 +6417,28 @@
     </row>
     <row r="131">
       <c r="A131" s="1" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="D131" s="1"/>
-      <c r="E131" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F131" s="2">
-        <v>68.0</v>
-      </c>
+        <v>334</v>
+      </c>
+      <c r="D131" s="2"/>
+      <c r="E131" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F131" s="3"/>
       <c r="G131" s="3"/>
       <c r="H131" s="9" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="I131" s="3"/>
       <c r="J131" s="3"/>
       <c r="K131" s="3"/>
       <c r="L131" s="3"/>
-      <c r="M131" s="2"/>
+      <c r="M131" s="3"/>
       <c r="N131" s="3"/>
       <c r="O131" s="3"/>
       <c r="P131" s="3"/>
@@ -6455,22 +6448,24 @@
     </row>
     <row r="132">
       <c r="A132" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B132" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="B132" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="C132" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="D132" s="2"/>
+      <c r="C132" s="46" t="s">
+        <v>336</v>
+      </c>
+      <c r="D132" s="10">
+        <v>36.0</v>
+      </c>
       <c r="E132" s="2" t="s">
         <v>62</v>
       </c>
       <c r="F132" s="3"/>
       <c r="G132" s="3"/>
       <c r="H132" s="9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I132" s="3"/>
       <c r="J132" s="3"/>
@@ -6486,23 +6481,26 @@
     </row>
     <row r="133">
       <c r="A133" s="1" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="C133" s="46" t="s">
-        <v>337</v>
-      </c>
-      <c r="D133" s="10">
-        <v>36.0</v>
-      </c>
-      <c r="E133" s="8" t="s">
-        <v>14</v>
+        <v>338</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D133" s="11">
+        <v>37.5</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F133" s="2">
+        <v>482.0</v>
       </c>
       <c r="G133" s="3"/>
       <c r="H133" s="9" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="I133" s="3"/>
       <c r="J133" s="3"/>
@@ -6518,26 +6516,22 @@
     </row>
     <row r="134">
       <c r="A134" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B134" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B134" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="D134" s="11">
-        <v>37.5</v>
-      </c>
+      <c r="C134" s="47" t="s">
+        <v>341</v>
+      </c>
+      <c r="D134" s="2"/>
       <c r="E134" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F134" s="2">
-        <v>482.0</v>
-      </c>
+        <v>342</v>
+      </c>
+      <c r="F134" s="2"/>
       <c r="G134" s="3"/>
       <c r="H134" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I134" s="3"/>
       <c r="J134" s="3"/>
@@ -6553,22 +6547,22 @@
     </row>
     <row r="135">
       <c r="A135" s="1" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="C135" s="47" t="s">
-        <v>342</v>
+        <v>95</v>
+      </c>
+      <c r="C135" s="39" t="s">
+        <v>344</v>
       </c>
       <c r="D135" s="2"/>
       <c r="E135" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="F135" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="F135" s="3"/>
       <c r="G135" s="3"/>
       <c r="H135" s="9" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="I135" s="3"/>
       <c r="J135" s="3"/>
@@ -6584,22 +6578,23 @@
     </row>
     <row r="136">
       <c r="A136" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C136" s="39" t="s">
-        <v>345</v>
-      </c>
-      <c r="D136" s="2"/>
+        <v>346</v>
+      </c>
       <c r="E136" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F136" s="3"/>
+        <v>73</v>
+      </c>
+      <c r="F136" s="2">
+        <v>82.0</v>
+      </c>
       <c r="G136" s="3"/>
       <c r="H136" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I136" s="3"/>
       <c r="J136" s="3"/>
@@ -6615,24 +6610,23 @@
     </row>
     <row r="137">
       <c r="A137" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C137" s="39" t="s">
+      <c r="C137" s="48" t="s">
         <v>347</v>
       </c>
-      <c r="D137" s="2"/>
-      <c r="E137" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F137" s="2">
-        <v>82.0</v>
+      <c r="D137" s="2">
+        <v>35.0</v>
+      </c>
+      <c r="E137" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="G137" s="3"/>
       <c r="H137" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I137" s="3"/>
       <c r="J137" s="3"/>
@@ -6648,22 +6642,24 @@
     </row>
     <row r="138">
       <c r="A138" s="1" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C138" s="48" t="s">
-        <v>348</v>
-      </c>
-      <c r="D138" s="2">
-        <v>35.0</v>
-      </c>
-      <c r="E138" s="2"/>
-      <c r="F138" s="2"/>
+        <v>349</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="D138" s="2"/>
+      <c r="E138" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F138" s="2">
+        <v>82.0</v>
+      </c>
       <c r="G138" s="3"/>
       <c r="H138" s="9" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="I138" s="3"/>
       <c r="J138" s="3"/>
@@ -6678,25 +6674,25 @@
       <c r="S138" s="3"/>
     </row>
     <row r="139">
-      <c r="A139" s="1" t="s">
+      <c r="A139" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B139" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B139" s="2" t="s">
-        <v>350</v>
-      </c>
       <c r="C139" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D139" s="2"/>
       <c r="E139" s="2" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="F139" s="2">
-        <v>82.0</v>
+        <v>964.0</v>
       </c>
       <c r="G139" s="3"/>
       <c r="H139" s="9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I139" s="3"/>
       <c r="J139" s="3"/>
@@ -6712,15 +6708,17 @@
     </row>
     <row r="140">
       <c r="A140" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B140" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B140" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="C140" s="2" t="s">
+      <c r="C140" s="48" t="s">
         <v>353</v>
       </c>
-      <c r="D140" s="2"/>
+      <c r="D140" s="2">
+        <v>42.0</v>
+      </c>
       <c r="E140" s="2" t="s">
         <v>29</v>
       </c>
@@ -6729,7 +6727,7 @@
       </c>
       <c r="G140" s="3"/>
       <c r="H140" s="9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I140" s="3"/>
       <c r="J140" s="3"/>
@@ -6744,14 +6742,14 @@
       <c r="S140" s="3"/>
     </row>
     <row r="141">
-      <c r="A141" s="1" t="s">
+      <c r="A141" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B141" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B141" s="2" t="s">
-        <v>350</v>
-      </c>
       <c r="C141" s="48" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D141" s="2">
         <v>42.0</v>
@@ -6764,7 +6762,7 @@
       </c>
       <c r="G141" s="3"/>
       <c r="H141" s="9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I141" s="3"/>
       <c r="J141" s="3"/>
@@ -6779,27 +6777,23 @@
       <c r="S141" s="3"/>
     </row>
     <row r="142">
-      <c r="A142" s="2" t="s">
+      <c r="A142" s="1" t="s">
         <v>355</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="C142" s="48" t="s">
-        <v>354</v>
-      </c>
-      <c r="D142" s="2">
-        <v>42.0</v>
-      </c>
+        <v>356</v>
+      </c>
+      <c r="C142" s="40" t="s">
+        <v>357</v>
+      </c>
+      <c r="D142" s="2"/>
       <c r="E142" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F142" s="2">
-        <v>964.0</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F142" s="3"/>
       <c r="G142" s="3"/>
       <c r="H142" s="9" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="I142" s="3"/>
       <c r="J142" s="3"/>
@@ -6815,22 +6809,24 @@
     </row>
     <row r="143">
       <c r="A143" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B143" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="B143" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="C143" s="40" t="s">
-        <v>358</v>
-      </c>
-      <c r="D143" s="2"/>
-      <c r="E143" s="2" t="s">
-        <v>18</v>
+      <c r="C143" s="35" t="s">
+        <v>359</v>
+      </c>
+      <c r="D143" s="2">
+        <v>22.8</v>
+      </c>
+      <c r="E143" s="30" t="s">
+        <v>360</v>
       </c>
       <c r="F143" s="3"/>
       <c r="G143" s="3"/>
       <c r="H143" s="9" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I143" s="3"/>
       <c r="J143" s="3"/>
@@ -6846,24 +6842,26 @@
     </row>
     <row r="144">
       <c r="A144" s="1" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="C144" s="35" t="s">
-        <v>360</v>
+        <v>362</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>363</v>
       </c>
       <c r="D144" s="2">
-        <v>22.8</v>
-      </c>
-      <c r="E144" s="30" t="s">
-        <v>361</v>
-      </c>
-      <c r="F144" s="3"/>
+        <v>34.5</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F144" s="2">
+        <v>31.0</v>
+      </c>
       <c r="G144" s="3"/>
       <c r="H144" s="9" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="I144" s="3"/>
       <c r="J144" s="3"/>
@@ -6878,14 +6876,14 @@
       <c r="S144" s="3"/>
     </row>
     <row r="145">
-      <c r="A145" s="1" t="s">
+      <c r="A145" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B145" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="C145" s="2" t="s">
         <v>363</v>
-      </c>
-      <c r="C145" s="2" t="s">
-        <v>364</v>
       </c>
       <c r="D145" s="2">
         <v>34.5</v>
@@ -6898,7 +6896,7 @@
       </c>
       <c r="G145" s="3"/>
       <c r="H145" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I145" s="3"/>
       <c r="J145" s="3"/>
@@ -6913,28 +6911,14 @@
       <c r="S145" s="3"/>
     </row>
     <row r="146">
-      <c r="A146" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="C146" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="D146" s="2">
-        <v>34.5</v>
-      </c>
-      <c r="E146" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F146" s="2">
-        <v>31.0</v>
-      </c>
+      <c r="A146" s="3"/>
+      <c r="B146" s="3"/>
+      <c r="C146" s="3"/>
+      <c r="D146" s="3"/>
+      <c r="E146" s="3"/>
+      <c r="F146" s="3"/>
       <c r="G146" s="3"/>
-      <c r="H146" s="9" t="s">
-        <v>365</v>
-      </c>
+      <c r="H146" s="3"/>
       <c r="I146" s="3"/>
       <c r="J146" s="3"/>
       <c r="K146" s="3"/>
@@ -6988,27 +6972,6 @@
       <c r="Q148" s="3"/>
       <c r="R148" s="3"/>
       <c r="S148" s="3"/>
-    </row>
-    <row r="149">
-      <c r="A149" s="3"/>
-      <c r="B149" s="3"/>
-      <c r="C149" s="3"/>
-      <c r="D149" s="3"/>
-      <c r="E149" s="3"/>
-      <c r="F149" s="3"/>
-      <c r="G149" s="3"/>
-      <c r="H149" s="3"/>
-      <c r="I149" s="3"/>
-      <c r="J149" s="3"/>
-      <c r="K149" s="3"/>
-      <c r="L149" s="3"/>
-      <c r="M149" s="3"/>
-      <c r="N149" s="3"/>
-      <c r="O149" s="3"/>
-      <c r="P149" s="3"/>
-      <c r="Q149" s="3"/>
-      <c r="R149" s="3"/>
-      <c r="S149" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="116">
@@ -7076,8 +7039,8 @@
     <mergeCell ref="H85:T85"/>
     <mergeCell ref="E90:F90"/>
     <mergeCell ref="E113:F113"/>
-    <mergeCell ref="E127:F127"/>
-    <mergeCell ref="E133:F133"/>
+    <mergeCell ref="E126:F126"/>
+    <mergeCell ref="E137:F137"/>
     <mergeCell ref="E96:F96"/>
     <mergeCell ref="E98:F98"/>
     <mergeCell ref="E101:F101"/>
@@ -7253,8 +7216,8 @@
     <hyperlink r:id="rId121" ref="H120"/>
     <hyperlink r:id="rId122" ref="H121"/>
     <hyperlink r:id="rId123" ref="H122"/>
-    <hyperlink r:id="rId124" ref="H123"/>
-    <hyperlink r:id="rId125" ref="C124"/>
+    <hyperlink r:id="rId124" ref="C123"/>
+    <hyperlink r:id="rId125" ref="H123"/>
     <hyperlink r:id="rId126" ref="H124"/>
     <hyperlink r:id="rId127" ref="H125"/>
     <hyperlink r:id="rId128" ref="H126"/>
@@ -7273,15 +7236,14 @@
     <hyperlink r:id="rId141" ref="H139"/>
     <hyperlink r:id="rId142" ref="H140"/>
     <hyperlink r:id="rId143" ref="H141"/>
-    <hyperlink r:id="rId144" ref="H142"/>
-    <hyperlink r:id="rId145" ref="C143"/>
-    <hyperlink r:id="rId146" ref="H143"/>
-    <hyperlink r:id="rId147" ref="E144"/>
+    <hyperlink r:id="rId144" ref="C142"/>
+    <hyperlink r:id="rId145" ref="H142"/>
+    <hyperlink r:id="rId146" ref="E143"/>
+    <hyperlink r:id="rId147" ref="H143"/>
     <hyperlink r:id="rId148" ref="H144"/>
     <hyperlink r:id="rId149" ref="H145"/>
-    <hyperlink r:id="rId150" ref="H146"/>
   </hyperlinks>
-  <drawing r:id="rId151"/>
+  <drawing r:id="rId150"/>
 </worksheet>
 </file>
 
@@ -7297,15 +7259,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>367</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3">
@@ -7325,12 +7287,12 @@
     </row>
     <row r="6">
       <c r="A6" s="30" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="30" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8">

</xml_diff>